<commit_message>
Syed - Steps updated in SiteStructureCommonSteps.java, CompartmentSwitchingTest.java, compartmentSwitchingTests.feature, onePassCompartmentSwitchingTests.feature  and sitestructure01/02 users added in CobaltUsers.xlsx
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C800138
</commit_message>
<xml_diff>
--- a/PPIUK-Phase2/PPIUK-SiteStructure/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-Phase2/PPIUK-SiteStructure/src/test/resources/CobaltUsers.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Emails" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="285">
   <si>
     <t>UserName</t>
   </si>
@@ -850,13 +850,35 @@
   </si>
   <si>
     <t>Global_page111!</t>
+  </si>
+  <si>
+    <t>sitestructure01</t>
+  </si>
+  <si>
+    <t>Password3</t>
+  </si>
+  <si>
+    <t>This is for only Site Structure Project</t>
+  </si>
+  <si>
+    <t>sitestructure01@mailinator.com</t>
+  </si>
+  <si>
+    <t>sitestructure02</t>
+  </si>
+  <si>
+    <t>sitestructure02@mailinator.com</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -952,7 +974,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -965,6 +987,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1026,7 +1049,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1061,7 +1084,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1270,20 +1293,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G115"/>
+  <dimension ref="A1:G117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="D115" sqref="D115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="40.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3389,6 +3412,40 @@
       </c>
       <c r="G115" s="10" t="s">
         <v>270</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="B116" t="s">
+        <v>279</v>
+      </c>
+      <c r="E116" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="F116" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G116" s="12" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="B117" t="s">
+        <v>279</v>
+      </c>
+      <c r="E117" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="F117" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G117" s="12" t="s">
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -3469,9 +3526,11 @@
     <hyperlink ref="G112" r:id="rId74"/>
     <hyperlink ref="G115" r:id="rId75"/>
     <hyperlink ref="G113" r:id="rId76" display="AssetPageUser1@mailinator.com "/>
+    <hyperlink ref="G116" r:id="rId77"/>
+    <hyperlink ref="G117" r:id="rId78"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId77"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId79"/>
 </worksheet>
 </file>
 
@@ -3485,8 +3544,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -3525,7 +3584,23 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>